<commit_message>
agregamos modulos de marcas, etiquetas y productos
</commit_message>
<xml_diff>
--- a/porcentajes-participacion.xlsx
+++ b/porcentajes-participacion.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Sam\universidad\8vo\Calidad de Software\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\universidad\8vo\Calidad de Software\gg\papa-noel-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFDD416D-DB92-47B8-BFD4-93BD6720AB9F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F9FF5DE-5C31-4A1A-A8D5-CE0AFB8AD61A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{686D8141-9220-4BED-BAA4-BD8EC43C11CC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{686D8141-9220-4BED-BAA4-BD8EC43C11CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="45">
   <si>
     <t>No entregó el primer trabajo, pero si los dos últimos y demostró interés en los trabajos finales</t>
   </si>
@@ -157,6 +158,9 @@
   </si>
   <si>
     <t>29 de mayo del 2019</t>
+  </si>
+  <si>
+    <t>15 de julio del 2019</t>
   </si>
 </sst>
 </file>
@@ -514,8 +518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2E6C7AF-B25B-428B-B103-B23F479F67F7}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection sqref="A1:E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -831,4 +835,299 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAC1C8DA-3A4A-47E9-A596-7DD2F9A4DADE}">
+  <dimension ref="A1:E24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="238.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A23:D23"/>
+    <mergeCell ref="A24:D24"/>
+    <mergeCell ref="A20:D20"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="A22:D22"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>